<commit_message>
updated NPM values for Guyana
</commit_message>
<xml_diff>
--- a/R/data/APT_data_corrected_April2025.xlsx
+++ b/R/data/APT_data_corrected_April2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gabrielle/Documents/RSE_gabrielle/93_VFSG/vfsg-apt/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{640E7563-CA99-0143-A345-0F6F71728450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB431221-0BAD-114B-B73E-04156A86C2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6223" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6222" uniqueCount="281">
   <si>
     <t>Region</t>
   </si>
@@ -1924,7 +1924,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1569"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1171" workbookViewId="0">
+      <selection activeCell="B1196" sqref="B1196"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -21409,12 +21411,8 @@
       <c r="C1196" s="65" t="s">
         <v>215</v>
       </c>
-      <c r="D1196" s="67" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1196" s="68">
-        <v>2012</v>
-      </c>
+      <c r="D1196" s="67"/>
+      <c r="E1196" s="68"/>
     </row>
     <row r="1197" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1197" s="63" t="s">

</xml_diff>